<commit_message>
Fix LCI of CHPs
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-combined-heat-power-plant-CCS.xlsx
+++ b/premise/data/additional_inventories/lci-combined-heat-power-plant-CCS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F2FD78-044E-C242-8612-9EECCE930C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A1C276-4BB5-7948-89CD-FF8715AB88EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,7 +597,7 @@
   <dimension ref="A1:K350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="K351" sqref="K351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1734,7 +1734,7 @@
         <v>23</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -5053,7 +5053,7 @@
         <v>23</v>
       </c>
       <c r="K322" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="323" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>